<commit_message>
Update course info (M2 IEAP ICDSP)
</commit_message>
<xml_diff>
--- a/data/M2-IEAP-ICDSP.xlsx
+++ b/data/M2-IEAP-ICDSP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/SSDS/enseignement/UFR STAPS/Direction/Outils/celcatreport/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7232DC9F-6BFE-0945-9832-42C74E6DAEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A01424-077F-D44F-8DA4-C8747AABCE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19700" xr2:uid="{154AE90F-D41B-8B49-BA91-D855BEB6F170}"/>
   </bookViews>
@@ -185,9 +185,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,464 +523,463 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D425352-B3D2-6642-82B3-EC9BD51219AA}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.5" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>311</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>20</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>20</v>
       </c>
-      <c r="H2" s="1">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>312</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="H3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>313</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1">
-        <v>10</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>321</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>5</v>
       </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>10</v>
-      </c>
-      <c r="J5" s="1">
-        <v>2</v>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>322</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>12</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>10</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2</v>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>323</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>16</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>25</v>
-      </c>
-      <c r="J7" s="1">
-        <v>2</v>
+      <c r="J7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>331</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>10</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8" s="1">
-        <v>2</v>
+      <c r="J8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>332</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
         <v>12</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>8</v>
       </c>
-      <c r="J9" s="1">
-        <v>2</v>
+      <c r="J9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>341</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>6</v>
       </c>
-      <c r="E10" s="1">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>30</v>
       </c>
-      <c r="H10" s="1">
-        <v>2</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
         <v>8</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>351</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>10</v>
-      </c>
-      <c r="J11" s="1">
-        <v>2</v>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>352</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>10</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12" s="1">
-        <v>2</v>
+      <c r="J12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>411</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
         <v>20</v>
       </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>10</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
-      <c r="I13" s="1">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>421</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>20</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>20</v>
       </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>10</v>
-      </c>
-      <c r="H14" s="1">
-        <v>2</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14">
         <v>3</v>
       </c>
     </row>

</xml_diff>